<commit_message>
update data source docs
</commit_message>
<xml_diff>
--- a/Data/data_source.xlsx
+++ b/Data/data_source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zehui\Desktop\Materials\Personal_docs\bikeshareTO_equity_analysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4369C82E-3085-4931-A083-1DF6F3B2871E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBC4FBB-F591-4767-8DDA-72EDE76DFB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -61,12 +61,6 @@
   </si>
   <si>
     <t>JSON</t>
-  </si>
-  <si>
-    <t>Toronto Parking Authority</t>
-  </si>
-  <si>
-    <t>through GBFS</t>
   </si>
   <si>
     <t>Road Network</t>
@@ -105,6 +99,9 @@
   </si>
   <si>
     <t>Statistics Canada through cancensus package (von Bergmann et al., 2021)</t>
+  </si>
+  <si>
+    <t>Toronto Parking Authority through GBFS</t>
   </si>
 </sst>
 </file>
@@ -508,9 +505,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -538,7 +537,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -555,93 +554,79 @@
         <v>45311</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="5">
+        <v>45299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="12">
+      <c r="B4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="12">
         <v>45299</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="12"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="12"/>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="4" t="s">
+    <row r="6" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="12">
-        <v>45299</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="1:5" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="D6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="9">
+      <c r="E6" s="9">
         <v>45327</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
+  <mergeCells count="4">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://open.toronto.ca/dataset/bike-share-toronto-ridership-data/" xr:uid="{476BF258-4273-44A8-B5E5-B6AE573F1A6E}"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://tor.publicbikesystem.net/ube/gbfs/v1/en/station_information" xr:uid="{847DFF3A-72F3-471B-9EF2-4770461052A8}"/>
-    <hyperlink ref="D4" r:id="rId3" display="https://tor.publicbikesystem.net/ube/gbfs/v1/en/station_information" xr:uid="{2DACE4A4-F3D7-4B82-BFD4-E1090140144D}"/>
-    <hyperlink ref="D5" r:id="rId4" display="https://download.geofabrik.de/north-america/canada/ontario.html" xr:uid="{21CA8973-D619-4F98-B07E-D58CE1BA1A7D}"/>
-    <hyperlink ref="D6" r:id="rId5" display="https://download.geofabrik.de/north-america/canada/ontario.html" xr:uid="{7C1408E2-109D-4D2C-8A86-19CCC74862B0}"/>
-    <hyperlink ref="D7" r:id="rId6" display="https://cran.r-project.org/web/packages/cancensus/index.html" xr:uid="{A3BCC6BA-099E-48EB-8CA8-B3C021022F71}"/>
+    <hyperlink ref="D4" r:id="rId2" display="https://download.geofabrik.de/north-america/canada/ontario.html" xr:uid="{21CA8973-D619-4F98-B07E-D58CE1BA1A7D}"/>
+    <hyperlink ref="D5" r:id="rId3" display="https://download.geofabrik.de/north-america/canada/ontario.html" xr:uid="{7C1408E2-109D-4D2C-8A86-19CCC74862B0}"/>
+    <hyperlink ref="D6" r:id="rId4" display="https://cran.r-project.org/web/packages/cancensus/index.html" xr:uid="{A3BCC6BA-099E-48EB-8CA8-B3C021022F71}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{3524FD72-3EBB-4F21-9ED8-0BDC0B1B6A30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update data source layout
</commit_message>
<xml_diff>
--- a/Data/data_source.xlsx
+++ b/Data/data_source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zehui\Desktop\Materials\Personal_docs\bikeshareTO_equity_analysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBC4FBB-F591-4767-8DDA-72EDE76DFB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A857CE-BBA4-4327-83C9-AA80DA45349B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -70,12 +70,6 @@
   </si>
   <si>
     <t>PBF</t>
-  </si>
-  <si>
-    <t>OpenStreetMap through</t>
-  </si>
-  <si>
-    <t>Geofabrik</t>
   </si>
   <si>
     <t>2021 Census</t>
@@ -103,12 +97,15 @@
   <si>
     <t>Toronto Parking Authority through GBFS</t>
   </si>
+  <si>
+    <t>OpenStreetMap through Geofabrik</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +140,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -186,7 +190,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -197,9 +201,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -209,21 +210,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -505,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +512,7 @@
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="41.140625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -547,14 +543,14 @@
       <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>45311</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -564,69 +560,68 @@
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="D3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="4">
         <v>45299</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="4">
+        <v>45299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="12">
-        <v>45299</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="D5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="9">
+      <c r="E5" s="7">
         <v>45327</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="E4:E5"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://open.toronto.ca/dataset/bike-share-toronto-ridership-data/" xr:uid="{476BF258-4273-44A8-B5E5-B6AE573F1A6E}"/>
-    <hyperlink ref="D4" r:id="rId2" display="https://download.geofabrik.de/north-america/canada/ontario.html" xr:uid="{21CA8973-D619-4F98-B07E-D58CE1BA1A7D}"/>
-    <hyperlink ref="D5" r:id="rId3" display="https://download.geofabrik.de/north-america/canada/ontario.html" xr:uid="{7C1408E2-109D-4D2C-8A86-19CCC74862B0}"/>
-    <hyperlink ref="D6" r:id="rId4" display="https://cran.r-project.org/web/packages/cancensus/index.html" xr:uid="{A3BCC6BA-099E-48EB-8CA8-B3C021022F71}"/>
-    <hyperlink ref="D3" r:id="rId5" xr:uid="{3524FD72-3EBB-4F21-9ED8-0BDC0B1B6A30}"/>
+    <hyperlink ref="D5" r:id="rId2" display="https://cran.r-project.org/web/packages/cancensus/index.html" xr:uid="{A3BCC6BA-099E-48EB-8CA8-B3C021022F71}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{3524FD72-3EBB-4F21-9ED8-0BDC0B1B6A30}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{F11BBA27-0D27-4C7A-A99F-64548E914FF6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>